<commit_message>
post request download excel
</commit_message>
<xml_diff>
--- a/files/test.xlsx
+++ b/files/test.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t xml:space="preserve">导出文件</t>
+    <t xml:space="preserve">测试采购单</t>
   </si>
   <si>
     <t xml:space="preserve">年</t>
@@ -67,43 +67,37 @@
     <t xml:space="preserve">签字</t>
   </si>
   <si>
-    <t xml:space="preserve">Fri Jul 06 2018 00:51:15 GMT+0800 (China Standard Time)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">瘦肉</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fri Jul 06 2018 00:51:15 GMT+0800 (China Standard Time)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fri Jul 06 2018 00:51:15 GMT+0800 (China Standard Time)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30</t>
+    <t xml:space="preserve">Sun Jul 08 2018 18:58:55 GMT+0800 (GMT+08:00)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">白菜</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">斤</t>
   </si>
   <si>
-    <t xml:space="preserve">15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">450</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sun Jul 08 2018 23:05:33 GMT+0800 (China Standard Time)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">瘦肉</t>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">采购人</t>
+  </si>
+  <si>
+    <t xml:space="preserve">收验货人</t>
+  </si>
+  <si>
+    <t xml:space="preserve">供货人</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sun Jul 08 2018 19:01:02 GMT+0800 (GMT+08:00)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">猪肉</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
@@ -112,10 +106,10 @@
     <t xml:space="preserve">斤</t>
   </si>
   <si>
-    <t xml:space="preserve">15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15</t>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
   </si>
   <si>
     <t xml:space="preserve">采购人</t>
@@ -127,10 +121,10 @@
     <t xml:space="preserve">供货人</t>
   </si>
   <si>
-    <t xml:space="preserve">Mon Jul 09 2018 23:43:52 GMT+0800 (China Standard Time)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">瘦肉</t>
+    <t xml:space="preserve">Sun Jul 08 2018 19:05:48 GMT+0800 (GMT+08:00)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">白菜</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
@@ -139,10 +133,10 @@
     <t xml:space="preserve">斤</t>
   </si>
   <si>
-    <t xml:space="preserve">15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15</t>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
   </si>
   <si>
     <t xml:space="preserve">采购人</t>
@@ -658,117 +652,113 @@
       <c r="B4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="J4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="K4" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="L4" s="4"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="J5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="K5" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="L5" s="4"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="J6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="K6" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>

</xml_diff>

<commit_message>
export select date, swipeout
</commit_message>
<xml_diff>
--- a/files/test.xlsx
+++ b/files/test.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t xml:space="preserve">测试采购单</t>
+    <t xml:space="preserve">龙场营镇者把小学学生营养餐食品原材料采购台账</t>
   </si>
   <si>
     <t xml:space="preserve">年</t>
@@ -67,10 +67,43 @@
     <t xml:space="preserve">签字</t>
   </si>
   <si>
-    <t xml:space="preserve">Sun Jul 08 2018 18:58:55 GMT+0800 (GMT+08:00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">白菜</t>
+    <t xml:space="preserve">Fri Jul 06 2018 00:51:15 GMT+0800 (China Standard Time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">瘦肉</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fri Jul 06 2018 00:51:15 GMT+0800 (China Standard Time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fri Jul 06 2018 00:51:15 GMT+0800 (China Standard Time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">斤</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sun Jul 08 2018 23:05:33 GMT+0800 (China Standard Time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">瘦肉</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
@@ -79,10 +112,10 @@
     <t xml:space="preserve">斤</t>
   </si>
   <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
   </si>
   <si>
     <t xml:space="preserve">采购人</t>
@@ -94,10 +127,10 @@
     <t xml:space="preserve">供货人</t>
   </si>
   <si>
-    <t xml:space="preserve">Sun Jul 08 2018 19:01:02 GMT+0800 (GMT+08:00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">猪肉</t>
+    <t xml:space="preserve">Mon Jul 09 2018 23:43:52 GMT+0800 (China Standard Time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">瘦肉</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
@@ -106,10 +139,10 @@
     <t xml:space="preserve">斤</t>
   </si>
   <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
   </si>
   <si>
     <t xml:space="preserve">采购人</t>
@@ -121,10 +154,10 @@
     <t xml:space="preserve">供货人</t>
   </si>
   <si>
-    <t xml:space="preserve">Sun Jul 08 2018 19:05:48 GMT+0800 (GMT+08:00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">白菜</t>
+    <t xml:space="preserve">Tue Jul 10 2018 23:10:06 GMT+0800 (China Standard Time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">瘦肉</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
@@ -133,10 +166,97 @@
     <t xml:space="preserve">斤</t>
   </si>
   <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">采购人</t>
+  </si>
+  <si>
+    <t xml:space="preserve">收验货人</t>
+  </si>
+  <si>
+    <t xml:space="preserve">供货人</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tue Jul 10 2018 23:13:14 GMT+0800 (China Standard Time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">瘦肉</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">斤</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">采购人</t>
+  </si>
+  <si>
+    <t xml:space="preserve">收验货人</t>
+  </si>
+  <si>
+    <t xml:space="preserve">供货人</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tue Jul 10 2018 23:13:31 GMT+0800 (China Standard Time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">瘦肉</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tue Jul 10 2018 23:45:44 GMT+0800 (China Standard Time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tue Jul 10 2018 23:45:46 GMT+0800 (China Standard Time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">斤</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">采购人</t>
+  </si>
+  <si>
+    <t xml:space="preserve">收验货人</t>
+  </si>
+  <si>
+    <t xml:space="preserve">供货人</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tue Jul 10 2018 23:45:36 GMT+0800 (China Standard Time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">瘦肉</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">斤</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
   </si>
   <si>
     <t xml:space="preserve">采购人</t>
@@ -652,116 +772,252 @@
       <c r="B4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="E4" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L4" s="4"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L5" s="4"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
+      <c r="A7" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2" t="s">
+      <c r="B7" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
     </row>
   </sheetData>
   <mergeCells>

</xml_diff>

<commit_message>
Export purchase details complete
</commit_message>
<xml_diff>
--- a/files/test.xlsx
+++ b/files/test.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t xml:space="preserve">龙场营镇者把小学学生营养餐食品原材料采购台账</t>
+    <t xml:space="preserve">学生营养餐食品原材料采购台账（第二个）</t>
   </si>
   <si>
     <t xml:space="preserve">                                             年  月份</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">签字</t>
   </si>
   <si>
-    <t xml:space="preserve">2018年09月27日</t>
+    <t xml:space="preserve">2018年09月28日</t>
   </si>
   <si>
     <t xml:space="preserve">猪肉</t>
@@ -82,13 +82,118 @@
     <t xml:space="preserve">14</t>
   </si>
   <si>
+    <t xml:space="preserve">Yuu</t>
+  </si>
+  <si>
     <t xml:space="preserve">123</t>
   </si>
   <si>
+    <t xml:space="preserve">2018年09月28日</t>
+  </si>
+  <si>
+    <t xml:space="preserve">猪肉</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018年09月28日</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">斤</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123123</t>
+  </si>
+  <si>
     <t xml:space="preserve">123</t>
   </si>
   <si>
     <t xml:space="preserve">123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018年09月28日</t>
+  </si>
+  <si>
+    <t xml:space="preserve">猪肉</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">斤</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018年09月28日</t>
+  </si>
+  <si>
+    <t xml:space="preserve">猪肉</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">斤</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018年09月28日</t>
+  </si>
+  <si>
+    <t xml:space="preserve">猪肉</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">斤</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1231</t>
   </si>
   <si>
     <t xml:space="preserve">    校长（签字）：             分管校长（签字）：              食堂管理员（签字）：                   监督员（签字）：                </t>
@@ -677,63 +782,189 @@
       <c r="I4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="7"/>
+      <c r="K4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" ht="30" customHeight="1">
+      <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" ht="19.5" customHeight="1">
-      <c r="A5" s="9" t="s">
+      <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
+      <c r="C5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" ht="30" customHeight="1">
+      <c r="A6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" ht="30" customHeight="1">
+      <c r="A7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" ht="30" customHeight="1">
+      <c r="A8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" ht="19.5" customHeight="1">
+      <c r="A9" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:L2"/>
-    <mergeCell ref="A5:L7"/>
+    <mergeCell ref="A9:L11"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.43263888888888902" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>